<commit_message>
Allow reading event parsing rules from a Config tab in the template spreadsheet. Instead of a 'weekly' section in the config file, use a parse_rules section, allowing name re-writing, weekly designation, and event time re-writing.  This configuration can also be read from the Config tab of the template.
</commit_message>
<xml_diff>
--- a/template/alternate.xlsx
+++ b/template/alternate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\diskstation\home\Drive\RubymineProjects\vh-events\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAE3349-2BB0-4F86-85B6-0D8DF62F746C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBD03BA-F67C-44FD-B727-C9F67AACFC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A40DE3AD-E031-4383-A1BB-AC0E2DF986DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A40DE3AD-E031-4383-A1BB-AC0E2DF986DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Day</t>
   </si>
@@ -114,10 +114,19 @@
     <t>village hall lunches</t>
   </si>
   <si>
-    <t>+15</t>
-  </si>
-  <si>
     <t>Circuit Training</t>
+  </si>
+  <si>
+    <t>Termtime only</t>
+  </si>
+  <si>
+    <t>+15-30</t>
+  </si>
+  <si>
+    <t>coffee shop</t>
+  </si>
+  <si>
+    <t>+45</t>
   </si>
 </sst>
 </file>
@@ -541,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE183364-5C8C-4586-AEB7-611D4AF4F133}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C14"/>
     </sheetView>
   </sheetViews>
@@ -571,7 +580,7 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -585,7 +594,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -654,10 +663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BA02AC-766F-419B-A84B-ABDB3B8F50D8}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,9 +674,10 @@
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
@@ -680,8 +690,11 @@
       <c r="D1" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -692,15 +705,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -708,15 +724,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -724,7 +743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -732,18 +751,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -751,7 +770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -759,12 +778,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>